<commit_message>
collab output title recip updated
</commit_message>
<xml_diff>
--- a/ArticleRecommendationProject/OutputFolder_Recommendations/Collaberative_Content_filtering_output.xlsx
+++ b/ArticleRecommendationProject/OutputFolder_Recommendations/Collaberative_Content_filtering_output.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7039" uniqueCount="4531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7040" uniqueCount="4532">
   <si>
     <t>Article</t>
   </si>
@@ -13613,6 +13613,9 @@
   </si>
   <si>
     <t>Rank</t>
+  </si>
+  <si>
+    <t>Recip</t>
   </si>
 </sst>
 </file>
@@ -14149,28 +14152,6 @@
   <dxfs count="5">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -14199,11 +14180,33 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="4"/>
+      <tableStyleElement type="headerRow" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -14472,7 +14475,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -14504,6 +14507,9 @@
       <c r="I1" t="s">
         <v>4530</v>
       </c>
+      <c r="J1" t="s">
+        <v>4531</v>
+      </c>
     </row>
     <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -18090,7 +18096,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>128</v>
       </c>
@@ -41988,13 +41994,13 @@
   </sheetData>
   <autoFilter ref="A1:J1033"/>
   <conditionalFormatting sqref="A1002:A1033">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1002:A1033">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1033">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "collab output title recip updated"
This reverts commit 174844c9c63a5b84ec72b3c5fe1a143a2681cec0.

testing revert
</commit_message>
<xml_diff>
--- a/ArticleRecommendationProject/OutputFolder_Recommendations/Collaberative_Content_filtering_output.xlsx
+++ b/ArticleRecommendationProject/OutputFolder_Recommendations/Collaberative_Content_filtering_output.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7040" uniqueCount="4532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7039" uniqueCount="4531">
   <si>
     <t>Article</t>
   </si>
@@ -13613,9 +13613,6 @@
   </si>
   <si>
     <t>Rank</t>
-  </si>
-  <si>
-    <t>Recip</t>
   </si>
 </sst>
 </file>
@@ -14152,6 +14149,28 @@
   <dxfs count="5">
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -14180,33 +14199,11 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="4"/>
-      <tableStyleElement type="headerRow" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -14475,7 +14472,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -14507,9 +14504,6 @@
       <c r="I1" t="s">
         <v>4530</v>
       </c>
-      <c r="J1" t="s">
-        <v>4531</v>
-      </c>
     </row>
     <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -18096,7 +18090,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>128</v>
       </c>
@@ -41994,13 +41988,13 @@
   </sheetData>
   <autoFilter ref="A1:J1033"/>
   <conditionalFormatting sqref="A1002:A1033">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1002:A1033">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1033">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>